<commit_message>
new and updated scripts
</commit_message>
<xml_diff>
--- a/data/main-codebook.xlsx
+++ b/data/main-codebook.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>url_article</t>
   </si>
@@ -44,9 +44,6 @@
     <t>comments</t>
   </si>
   <si>
-    <t>paper_id</t>
-  </si>
-  <si>
     <t>journal_id</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>n5_rep</t>
   </si>
   <si>
-    <t>mi_rep</t>
-  </si>
-  <si>
     <t>mitest_rep</t>
   </si>
   <si>
@@ -177,6 +171,9 @@
   </si>
   <si>
     <t>power</t>
+  </si>
+  <si>
+    <t>article_id</t>
   </si>
 </sst>
 </file>
@@ -582,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AY104"/>
+  <dimension ref="A1:AX104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AR9" sqref="AR9"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AR8" sqref="AR8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,16 +609,16 @@
     <col min="37" max="37" width="17.140625" customWidth="1"/>
     <col min="38" max="38" width="18" customWidth="1"/>
     <col min="39" max="39" width="20.85546875" style="7" customWidth="1"/>
-    <col min="50" max="50" width="13.5703125" customWidth="1"/>
-    <col min="51" max="51" width="14" customWidth="1"/>
+    <col min="49" max="49" width="13.5703125" customWidth="1"/>
+    <col min="50" max="50" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -630,13 +627,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>2</v>
@@ -645,133 +642,130 @@
         <v>3</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AO1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AT1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AU1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AJ1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK1" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AM1" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="AN1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AO1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AP1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AQ1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AR1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AS1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AT1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AU1" s="3" t="s">
+      <c r="AV1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AV1" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="AW1" s="3" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="AX1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="AY1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="C2" s="8"/>
     </row>
     <row r="45" spans="17:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
final files for main study
</commit_message>
<xml_diff>
--- a/data/main-codebook.xlsx
+++ b/data/main-codebook.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>url_article</t>
   </si>
@@ -53,9 +53,6 @@
     <t>author</t>
   </si>
   <si>
-    <t>title</t>
-  </si>
-  <si>
     <t>type_group</t>
   </si>
   <si>
@@ -149,9 +146,6 @@
     <t>data_usability</t>
   </si>
   <si>
-    <t>compare_groups</t>
-  </si>
-  <si>
     <t>n_res</t>
   </si>
   <si>
@@ -174,24 +168,19 @@
   </si>
   <si>
     <t>article_id</t>
+  </si>
+  <si>
+    <t>compare_group</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -228,7 +217,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -270,33 +259,33 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -579,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AX104"/>
+  <dimension ref="A1:AW104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AR8" sqref="AR8"/>
+    <sheetView tabSelected="1" topLeftCell="AQ1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AT5" sqref="AT5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,191 +580,187 @@
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
     <col min="6" max="6" width="37.7109375" customWidth="1"/>
-    <col min="7" max="7" width="44.7109375" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" customWidth="1"/>
-    <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
     <col min="14" max="14" width="17.140625" customWidth="1"/>
     <col min="15" max="15" width="16.140625" customWidth="1"/>
     <col min="16" max="16" width="14.5703125" customWidth="1"/>
     <col min="17" max="17" width="16.140625" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" customWidth="1"/>
-    <col min="19" max="19" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="17.140625" customWidth="1"/>
-    <col min="33" max="33" width="16.7109375" customWidth="1"/>
-    <col min="34" max="34" width="15.85546875" customWidth="1"/>
-    <col min="35" max="35" width="17" customWidth="1"/>
-    <col min="36" max="36" width="14.5703125" customWidth="1"/>
-    <col min="37" max="37" width="17.140625" customWidth="1"/>
-    <col min="38" max="38" width="18" customWidth="1"/>
-    <col min="39" max="39" width="20.85546875" style="7" customWidth="1"/>
-    <col min="49" max="49" width="13.5703125" customWidth="1"/>
-    <col min="50" max="50" width="14" customWidth="1"/>
+    <col min="18" max="18" width="6.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.140625" customWidth="1"/>
+    <col min="32" max="32" width="16.7109375" customWidth="1"/>
+    <col min="33" max="33" width="15.85546875" customWidth="1"/>
+    <col min="34" max="34" width="17" customWidth="1"/>
+    <col min="35" max="35" width="14.5703125" customWidth="1"/>
+    <col min="36" max="36" width="17.140625" customWidth="1"/>
+    <col min="37" max="37" width="18" customWidth="1"/>
+    <col min="38" max="38" width="20.85546875" style="4" customWidth="1"/>
+    <col min="48" max="48" width="13.5703125" customWidth="1"/>
+    <col min="49" max="49" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:49" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AK1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AO1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AP1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR1" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="AS1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AJ1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AK1" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AM1" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="AN1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AO1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AP1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AQ1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AR1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AS1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AT1" s="3" t="s">
+      <c r="AT1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="AU1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AV1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AW1" s="3" t="s">
+      <c r="AV1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="AX1" s="3" t="s">
+      <c r="AW1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="C2" s="8"/>
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="C2" s="5"/>
     </row>
     <row r="45" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q45" s="4"/>
+      <c r="Q45" s="2"/>
     </row>
     <row r="46" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q46" s="4"/>
+      <c r="Q46" s="2"/>
     </row>
-    <row r="104" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R104" s="5"/>
+    <row r="104" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M104" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>